<commit_message>
logros reporte se agrego usuarios
</commit_message>
<xml_diff>
--- a/backend/resources/templates/reporte_logros.xlsx
+++ b/backend/resources/templates/reporte_logros.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Periodo del POI</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>IV Trimestre</t>
+  </si>
+  <si>
+    <t>USUARIO</t>
   </si>
 </sst>
 </file>
@@ -276,17 +279,17 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -316,7 +319,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4049062</xdr:colOff>
+      <xdr:colOff>2280133</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>79012</xdr:rowOff>
     </xdr:to>
@@ -325,7 +328,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99E84EB8-DC54-4CDB-B5F3-0487DD1E8A22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{99E84EB8-DC54-4CDB-B5F3-0487DD1E8A22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -617,115 +620,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R14"/>
+  <dimension ref="B2:S14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="11"/>
-    <col min="2" max="2" width="23.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="97" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="100.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="41.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="116.42578125" style="14" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" style="10" customWidth="1"/>
-    <col min="15" max="18" width="35.7109375" style="10" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="11"/>
+    <col min="2" max="2" width="50.28515625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="39" style="9" customWidth="1"/>
+    <col min="4" max="4" width="97" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="116.42578125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" style="10" customWidth="1"/>
+    <col min="16" max="19" width="35.7109375" style="10" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="23"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="2"/>
-      <c r="K2" s="3"/>
+    <row r="2" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="22"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="2"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="15"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="3"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
-    </row>
-    <row r="3" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="2"/>
-      <c r="K3" s="3"/>
+      <c r="S2" s="15"/>
+    </row>
+    <row r="3" spans="2:19" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="C3" s="4"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="2"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="15"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="3"/>
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
-    </row>
-    <row r="4" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="23"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="2"/>
-      <c r="K4" s="3"/>
+      <c r="S3" s="15"/>
+    </row>
+    <row r="4" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="22"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="2"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="15"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="3"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
-    </row>
-    <row r="5" spans="2:18" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+      <c r="S4" s="15"/>
+    </row>
+    <row r="5" spans="2:19" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="6"/>
-      <c r="K5" s="8"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="6"/>
       <c r="L5" s="8"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="16"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="8"/>
       <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
-    </row>
-    <row r="6" spans="2:18" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="C6" s="24"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="6"/>
-      <c r="K6" s="8"/>
+      <c r="S5" s="16"/>
+    </row>
+    <row r="6" spans="2:19" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="D6" s="23"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="6"/>
       <c r="L6" s="8"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="16"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="8"/>
       <c r="P6" s="16"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
-    </row>
-    <row r="7" spans="2:18" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="S6" s="16"/>
+    </row>
+    <row r="7" spans="2:19" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="24">
         <v>2024</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="24"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="6"/>
       <c r="M7" s="6"/>
       <c r="O7" s="17"/>
@@ -733,15 +737,15 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
     </row>
-    <row r="8" spans="2:18" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:19" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="24"/>
+      <c r="E8" s="23"/>
       <c r="F8" s="6"/>
       <c r="M8" s="6"/>
       <c r="O8" s="17"/>
@@ -749,15 +753,15 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
     </row>
-    <row r="9" spans="2:18" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:19" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B9" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="24"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="6"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -768,15 +772,15 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
     </row>
-    <row r="10" spans="2:18" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:19" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="24" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="24"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="6"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
@@ -787,15 +791,15 @@
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
     </row>
-    <row r="11" spans="2:18" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:19" s="7" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="24"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="6"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
@@ -806,28 +810,29 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
     </row>
-    <row r="12" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-    </row>
-    <row r="13" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="19"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="11"/>
+    </row>
+    <row r="13" spans="2:19" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
@@ -839,57 +844,61 @@
       <c r="P13" s="19"/>
       <c r="Q13" s="19"/>
       <c r="R13" s="19"/>
-    </row>
-    <row r="14" spans="2:18" s="12" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S13" s="19"/>
+    </row>
+    <row r="14" spans="2:19" s="12" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="D14" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="E14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="F14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="G14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="H14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="I14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="J14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="K14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="L14" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="M14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M14" s="13" t="s">
+      <c r="N14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="13" t="s">
+      <c r="O14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="O14" s="18" t="s">
+      <c r="P14" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="P14" s="18" t="s">
+      <c r="Q14" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="Q14" s="18" t="s">
+      <c r="R14" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="R14" s="18" t="s">
+      <c r="S14" s="18" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>